<commit_message>
Starting incorperate chemical database to remove redudant information in experiment plan
</commit_message>
<xml_diff>
--- a/PlanPrepareProcess/Chemical Database.xlsx
+++ b/PlanPrepareProcess/Chemical Database.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Desktop\OT2-DOE\PlanPrepareProcess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB07A6F-6510-46E9-9B27-7016C19054F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="20325" windowHeight="16725" xr2:uid="{C2D02F0C-41A0-499C-990D-9384FF3DDD2C}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="20325" windowHeight="16725"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Component Full Name</t>
   </si>
@@ -94,12 +93,24 @@
   </si>
   <si>
     <t>Negligible</t>
+  </si>
+  <si>
+    <t>cadmiumoleate</t>
+  </si>
+  <si>
+    <t>topselenide</t>
+  </si>
+  <si>
+    <t>Cadmium Oleate</t>
+  </si>
+  <si>
+    <t>Triphenylphosphine selenide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,11 +455,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C65780-6C0F-4505-92CE-2B417DAE6D35}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +569,34 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>675.3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>341.3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>